<commit_message>
Code has been updated, Sample Page Object has been added
</commit_message>
<xml_diff>
--- a/WithSelenium/WebAutomation/OnJava_WithTestNG/src/org/nng/test/datafiles/TestData.xlsx
+++ b/WithSelenium/WebAutomation/OnJava_WithTestNG/src/org/nng/test/datafiles/TestData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="15420" windowHeight="5040"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="15420" windowHeight="5040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sample1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Case1_GoogleSearch" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>PASSWORD</t>
   </si>
@@ -359,13 +359,25 @@
   </si>
   <si>
     <t>1000004</t>
+  </si>
+  <si>
+    <t>Google Search Keywords</t>
+  </si>
+  <si>
+    <t>No of Result listed</t>
+  </si>
+  <si>
+    <t>Times(Frequency)</t>
+  </si>
+  <si>
+    <t>Date and Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +424,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -432,7 +452,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -455,16 +475,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -488,9 +518,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -786,7 +818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -878,12 +910,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1">
+      <c r="A1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>